<commit_message>
chore: update deps and data
</commit_message>
<xml_diff>
--- a/data/GreatLink/GreatLink Asia Dividend Advantage.xlsx
+++ b/data/GreatLink/GreatLink Asia Dividend Advantage.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="PriceHistory" sheetId="1" r:id="GemRid281025"/>
+    <sheet name="PriceHistory" sheetId="1" r:id="GemRid242318"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="321">
   <si>
     <t>Price Date</t>
   </si>
@@ -26,15 +26,93 @@
     <t>Currency - Unit Level</t>
   </si>
   <si>
+    <t>07/04/2025</t>
+  </si>
+  <si>
+    <t>0.866</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>04/04/2025</t>
+  </si>
+  <si>
+    <t>0.936</t>
+  </si>
+  <si>
+    <t>03/04/2025</t>
+  </si>
+  <si>
+    <t>02/04/2025</t>
+  </si>
+  <si>
+    <t>0.972</t>
+  </si>
+  <si>
+    <t>01/04/2025</t>
+  </si>
+  <si>
+    <t>0.968</t>
+  </si>
+  <si>
+    <t>28/03/2025</t>
+  </si>
+  <si>
+    <t>0.975</t>
+  </si>
+  <si>
+    <t>27/03/2025</t>
+  </si>
+  <si>
+    <t>0.978</t>
+  </si>
+  <si>
+    <t>26/03/2025</t>
+  </si>
+  <si>
+    <t>0.976</t>
+  </si>
+  <si>
+    <t>25/03/2025</t>
+  </si>
+  <si>
+    <t>0.969</t>
+  </si>
+  <si>
+    <t>24/03/2025</t>
+  </si>
+  <si>
+    <t>21/03/2025</t>
+  </si>
+  <si>
+    <t>20/03/2025</t>
+  </si>
+  <si>
+    <t>0.973</t>
+  </si>
+  <si>
+    <t>19/03/2025</t>
+  </si>
+  <si>
+    <t>18/03/2025</t>
+  </si>
+  <si>
+    <t>17/03/2025</t>
+  </si>
+  <si>
+    <t>0.957</t>
+  </si>
+  <si>
+    <t>14/03/2025</t>
+  </si>
+  <si>
     <t>13/03/2025</t>
   </si>
   <si>
     <t>0.950</t>
   </si>
   <si>
-    <t>SGD</t>
-  </si>
-  <si>
     <t>12/03/2025</t>
   </si>
   <si>
@@ -80,15 +158,9 @@
     <t>27/02/2025</t>
   </si>
   <si>
-    <t>0.975</t>
-  </si>
-  <si>
     <t>26/02/2025</t>
   </si>
   <si>
-    <t>0.968</t>
-  </si>
-  <si>
     <t>25/02/2025</t>
   </si>
   <si>
@@ -104,9 +176,6 @@
     <t>21/02/2025</t>
   </si>
   <si>
-    <t>0.978</t>
-  </si>
-  <si>
     <t>20/02/2025</t>
   </si>
   <si>
@@ -200,9 +269,6 @@
     <t>16/01/2025</t>
   </si>
   <si>
-    <t>0.957</t>
-  </si>
-  <si>
     <t>15/01/2025</t>
   </si>
   <si>
@@ -233,15 +299,9 @@
     <t>07/01/2025</t>
   </si>
   <si>
-    <t>0.973</t>
-  </si>
-  <si>
     <t>06/01/2025</t>
   </si>
   <si>
-    <t>0.972</t>
-  </si>
-  <si>
     <t>03/01/2025</t>
   </si>
   <si>
@@ -383,15 +443,9 @@
     <t>20/11/2024</t>
   </si>
   <si>
-    <t>0.976</t>
-  </si>
-  <si>
     <t>19/11/2024</t>
   </si>
   <si>
-    <t>0.969</t>
-  </si>
-  <si>
     <t>18/11/2024</t>
   </si>
   <si>
@@ -642,9 +696,6 @@
   </si>
   <si>
     <t>21/08/2024</t>
-  </si>
-  <si>
-    <t>0.936</t>
   </si>
   <si>
     <t>20/08/2024</t>
@@ -1293,7 +1344,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1301,10 +1352,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1312,10 +1363,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1323,10 +1374,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1334,10 +1385,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -1348,7 +1399,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1356,10 +1407,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -1367,10 +1418,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1378,10 +1429,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1389,10 +1440,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1400,10 +1451,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1414,7 +1465,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1422,10 +1473,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -1433,10 +1484,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1444,10 +1495,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
         <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -1455,10 +1506,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1466,10 +1517,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -1480,7 +1531,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -1488,10 +1539,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1499,10 +1550,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -1510,10 +1561,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -1521,10 +1572,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -1532,10 +1583,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -1543,10 +1594,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -1554,10 +1605,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1565,10 +1616,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -1576,10 +1627,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -1587,10 +1638,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
@@ -1598,10 +1649,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -1609,10 +1660,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1620,10 +1671,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -1631,10 +1682,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -1642,10 +1693,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -1653,10 +1704,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -1664,10 +1715,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -1675,10 +1726,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -1686,10 +1737,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -1697,10 +1748,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -1708,10 +1759,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -1719,10 +1770,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -1730,10 +1781,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -1741,10 +1792,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1752,10 +1803,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1763,10 +1814,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
         <v>71</v>
-      </c>
-      <c r="B47" t="s">
-        <v>72</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1777,7 +1828,7 @@
         <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1785,10 +1836,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" t="s">
         <v>75</v>
-      </c>
-      <c r="B49" t="s">
-        <v>76</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1796,10 +1847,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" t="s">
         <v>77</v>
-      </c>
-      <c r="B50" t="s">
-        <v>78</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -1807,10 +1858,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1818,10 +1869,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -1829,10 +1880,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1840,10 +1891,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -1851,10 +1902,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -1862,10 +1913,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -1873,10 +1924,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1884,10 +1935,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -1895,10 +1946,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B59" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1906,10 +1957,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -1917,10 +1968,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -1928,10 +1979,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1939,10 +1990,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -1950,10 +2001,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -1961,10 +2012,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B65" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -1972,10 +2023,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -1983,10 +2034,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -1994,10 +2045,10 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -2005,10 +2056,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B69" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
@@ -2016,10 +2067,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B70" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -2027,10 +2078,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -2038,10 +2089,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -2049,10 +2100,10 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
@@ -2060,10 +2111,10 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B74" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
@@ -2071,10 +2122,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
@@ -2082,10 +2133,10 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B76" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="C76" t="s">
         <v>5</v>
@@ -2093,10 +2144,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C77" t="s">
         <v>5</v>
@@ -2104,10 +2155,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B78" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="C78" t="s">
         <v>5</v>
@@ -2115,10 +2166,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B79" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C79" t="s">
         <v>5</v>
@@ -2126,10 +2177,10 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B80" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -2137,10 +2188,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B81" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C81" t="s">
         <v>5</v>
@@ -2148,10 +2199,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B82" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
@@ -2159,10 +2210,10 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B83" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
@@ -2170,10 +2221,10 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B84" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C84" t="s">
         <v>5</v>
@@ -2181,10 +2232,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B85" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
       <c r="C85" t="s">
         <v>5</v>
@@ -2192,10 +2243,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B86" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="C86" t="s">
         <v>5</v>
@@ -2203,10 +2254,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B87" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C87" t="s">
         <v>5</v>
@@ -2214,10 +2265,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="C88" t="s">
         <v>5</v>
@@ -2225,10 +2276,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B89" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
@@ -2236,10 +2287,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B90" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="C90" t="s">
         <v>5</v>
@@ -2247,10 +2298,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
@@ -2258,10 +2309,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B92" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C92" t="s">
         <v>5</v>
@@ -2269,10 +2320,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="C93" t="s">
         <v>5</v>
@@ -2280,10 +2331,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B94" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
@@ -2291,10 +2342,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B95" t="s">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="C95" t="s">
         <v>5</v>
@@ -2302,10 +2353,10 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B96" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -2313,10 +2364,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B97" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
@@ -2324,10 +2375,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B98" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="C98" t="s">
         <v>5</v>
@@ -2335,10 +2386,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B99" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
@@ -2346,10 +2397,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B100" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>
@@ -2357,10 +2408,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B101" t="s">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="C101" t="s">
         <v>5</v>
@@ -2368,10 +2419,10 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
+        <v>150</v>
+      </c>
+      <c r="B102" t="s">
         <v>151</v>
-      </c>
-      <c r="B102" t="s">
-        <v>15</v>
       </c>
       <c r="C102" t="s">
         <v>5</v>
@@ -2382,7 +2433,7 @@
         <v>152</v>
       </c>
       <c r="B103" t="s">
-        <v>29</v>
+        <v>153</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
@@ -2390,10 +2441,10 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B104" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C104" t="s">
         <v>5</v>
@@ -2401,10 +2452,10 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B105" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="C105" t="s">
         <v>5</v>
@@ -2415,7 +2466,7 @@
         <v>156</v>
       </c>
       <c r="B106" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="C106" t="s">
         <v>5</v>
@@ -2426,7 +2477,7 @@
         <v>157</v>
       </c>
       <c r="B107" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="C107" t="s">
         <v>5</v>
@@ -2437,7 +2488,7 @@
         <v>158</v>
       </c>
       <c r="B108" t="s">
-        <v>133</v>
+        <v>41</v>
       </c>
       <c r="C108" t="s">
         <v>5</v>
@@ -2448,7 +2499,7 @@
         <v>159</v>
       </c>
       <c r="B109" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="C109" t="s">
         <v>5</v>
@@ -2470,7 +2521,7 @@
         <v>162</v>
       </c>
       <c r="B111" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="C111" t="s">
         <v>5</v>
@@ -2481,7 +2532,7 @@
         <v>163</v>
       </c>
       <c r="B112" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="C112" t="s">
         <v>5</v>
@@ -2492,7 +2543,7 @@
         <v>164</v>
       </c>
       <c r="B113" t="s">
-        <v>165</v>
+        <v>108</v>
       </c>
       <c r="C113" t="s">
         <v>5</v>
@@ -2500,10 +2551,10 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B114" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="C114" t="s">
         <v>5</v>
@@ -2511,10 +2562,10 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B115" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C115" t="s">
         <v>5</v>
@@ -2522,10 +2573,10 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B116" t="s">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="C116" t="s">
         <v>5</v>
@@ -2533,10 +2584,10 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B117" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
       <c r="C117" t="s">
         <v>5</v>
@@ -2544,10 +2595,10 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B118" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C118" t="s">
         <v>5</v>
@@ -2555,10 +2606,10 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B119" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="C119" t="s">
         <v>5</v>
@@ -2566,10 +2617,10 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B120" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="C120" t="s">
         <v>5</v>
@@ -2577,10 +2628,10 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
+        <v>172</v>
+      </c>
+      <c r="B121" t="s">
         <v>173</v>
-      </c>
-      <c r="B121" t="s">
-        <v>7</v>
       </c>
       <c r="C121" t="s">
         <v>5</v>
@@ -2591,7 +2642,7 @@
         <v>174</v>
       </c>
       <c r="B122" t="s">
-        <v>175</v>
+        <v>111</v>
       </c>
       <c r="C122" t="s">
         <v>5</v>
@@ -2599,10 +2650,10 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B123" t="s">
-        <v>177</v>
+        <v>124</v>
       </c>
       <c r="C123" t="s">
         <v>5</v>
@@ -2610,10 +2661,10 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B124" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="C124" t="s">
         <v>5</v>
@@ -2621,10 +2672,10 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B125" t="s">
-        <v>181</v>
+        <v>98</v>
       </c>
       <c r="C125" t="s">
         <v>5</v>
@@ -2632,10 +2683,10 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B126" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C126" t="s">
         <v>5</v>
@@ -2643,10 +2694,10 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B127" t="s">
-        <v>181</v>
+        <v>119</v>
       </c>
       <c r="C127" t="s">
         <v>5</v>
@@ -2654,10 +2705,10 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B128" t="s">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="C128" t="s">
         <v>5</v>
@@ -2665,10 +2716,10 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B129" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C129" t="s">
         <v>5</v>
@@ -2676,10 +2727,10 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B130" t="s">
-        <v>189</v>
+        <v>115</v>
       </c>
       <c r="C130" t="s">
         <v>5</v>
@@ -2687,10 +2738,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B131" t="s">
-        <v>187</v>
+        <v>115</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -2698,10 +2749,10 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B132" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="C132" t="s">
         <v>5</v>
@@ -2709,10 +2760,10 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B133" t="s">
-        <v>192</v>
+        <v>100</v>
       </c>
       <c r="C133" t="s">
         <v>5</v>
@@ -2720,10 +2771,10 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B134" t="s">
-        <v>195</v>
+        <v>12</v>
       </c>
       <c r="C134" t="s">
         <v>5</v>
@@ -2731,10 +2782,10 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B135" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="C135" t="s">
         <v>5</v>
@@ -2742,10 +2793,10 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B136" t="s">
-        <v>195</v>
+        <v>77</v>
       </c>
       <c r="C136" t="s">
         <v>5</v>
@@ -2753,10 +2804,10 @@
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B137" t="s">
-        <v>175</v>
+        <v>33</v>
       </c>
       <c r="C137" t="s">
         <v>5</v>
@@ -2764,10 +2815,10 @@
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B138" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C138" t="s">
         <v>5</v>
@@ -2775,10 +2826,10 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B139" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C139" t="s">
         <v>5</v>
@@ -2786,10 +2837,10 @@
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B140" t="s">
-        <v>52</v>
+        <v>197</v>
       </c>
       <c r="C140" t="s">
         <v>5</v>
@@ -2797,10 +2848,10 @@
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B141" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C141" t="s">
         <v>5</v>
@@ -2808,10 +2859,10 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B142" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C142" t="s">
         <v>5</v>
@@ -2819,10 +2870,10 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B143" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C143" t="s">
         <v>5</v>
@@ -2830,10 +2881,10 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B144" t="s">
-        <v>52</v>
+        <v>203</v>
       </c>
       <c r="C144" t="s">
         <v>5</v>
@@ -2841,10 +2892,10 @@
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B145" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C145" t="s">
         <v>5</v>
@@ -2852,10 +2903,10 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B146" t="s">
-        <v>175</v>
+        <v>207</v>
       </c>
       <c r="C146" t="s">
         <v>5</v>
@@ -2863,10 +2914,10 @@
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B147" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="C147" t="s">
         <v>5</v>
@@ -2874,10 +2925,10 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B148" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C148" t="s">
         <v>5</v>
@@ -2885,10 +2936,10 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B149" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C149" t="s">
         <v>5</v>
@@ -2896,10 +2947,10 @@
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B150" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="C150" t="s">
         <v>5</v>
@@ -2907,10 +2958,10 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B151" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="C151" t="s">
         <v>5</v>
@@ -2918,10 +2969,10 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B152" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C152" t="s">
         <v>5</v>
@@ -2929,10 +2980,10 @@
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B153" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="C153" t="s">
         <v>5</v>
@@ -2940,10 +2991,10 @@
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B154" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="C154" t="s">
         <v>5</v>
@@ -2951,10 +3002,10 @@
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B155" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="C155" t="s">
         <v>5</v>
@@ -2962,10 +3013,10 @@
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B156" t="s">
-        <v>228</v>
+        <v>75</v>
       </c>
       <c r="C156" t="s">
         <v>5</v>
@@ -2973,10 +3024,10 @@
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B157" t="s">
-        <v>66</v>
+        <v>223</v>
       </c>
       <c r="C157" t="s">
         <v>5</v>
@@ -2984,10 +3035,10 @@
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B158" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="C158" t="s">
         <v>5</v>
@@ -2995,10 +3046,10 @@
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B159" t="s">
-        <v>232</v>
+        <v>7</v>
       </c>
       <c r="C159" t="s">
         <v>5</v>
@@ -3006,10 +3057,10 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B160" t="s">
-        <v>234</v>
+        <v>75</v>
       </c>
       <c r="C160" t="s">
         <v>5</v>
@@ -3017,10 +3068,10 @@
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B161" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="C161" t="s">
         <v>5</v>
@@ -3028,10 +3079,10 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B162" t="s">
-        <v>7</v>
+        <v>193</v>
       </c>
       <c r="C162" t="s">
         <v>5</v>
@@ -3039,10 +3090,10 @@
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B163" t="s">
-        <v>23</v>
+        <v>210</v>
       </c>
       <c r="C163" t="s">
         <v>5</v>
@@ -3050,10 +3101,10 @@
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B164" t="s">
-        <v>23</v>
+        <v>232</v>
       </c>
       <c r="C164" t="s">
         <v>5</v>
@@ -3061,10 +3112,10 @@
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B165" t="s">
-        <v>23</v>
+        <v>234</v>
       </c>
       <c r="C165" t="s">
         <v>5</v>
@@ -3072,10 +3123,10 @@
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B166" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
       <c r="C166" t="s">
         <v>5</v>
@@ -3083,10 +3134,10 @@
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B167" t="s">
-        <v>143</v>
+        <v>237</v>
       </c>
       <c r="C167" t="s">
         <v>5</v>
@@ -3094,10 +3145,10 @@
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B168" t="s">
-        <v>76</v>
+        <v>239</v>
       </c>
       <c r="C168" t="s">
         <v>5</v>
@@ -3105,10 +3156,10 @@
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B169" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C169" t="s">
         <v>5</v>
@@ -3116,10 +3167,10 @@
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B170" t="s">
-        <v>80</v>
+        <v>203</v>
       </c>
       <c r="C170" t="s">
         <v>5</v>
@@ -3127,10 +3178,10 @@
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B171" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="C171" t="s">
         <v>5</v>
@@ -3138,10 +3189,10 @@
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B172" t="s">
-        <v>34</v>
+        <v>245</v>
       </c>
       <c r="C172" t="s">
         <v>5</v>
@@ -3149,10 +3200,10 @@
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B173" t="s">
-        <v>249</v>
+        <v>88</v>
       </c>
       <c r="C173" t="s">
         <v>5</v>
@@ -3160,10 +3211,10 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B174" t="s">
-        <v>29</v>
+        <v>220</v>
       </c>
       <c r="C174" t="s">
         <v>5</v>
@@ -3171,10 +3222,10 @@
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B175" t="s">
-        <v>117</v>
+        <v>249</v>
       </c>
       <c r="C175" t="s">
         <v>5</v>
@@ -3182,10 +3233,10 @@
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B176" t="s">
-        <v>112</v>
+        <v>251</v>
       </c>
       <c r="C176" t="s">
         <v>5</v>
@@ -3193,10 +3244,10 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B177" t="s">
-        <v>122</v>
+        <v>225</v>
       </c>
       <c r="C177" t="s">
         <v>5</v>
@@ -3204,10 +3255,10 @@
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B178" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C178" t="s">
         <v>5</v>
@@ -3215,10 +3266,10 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B179" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="C179" t="s">
         <v>5</v>
@@ -3226,10 +3277,10 @@
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B180" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="C180" t="s">
         <v>5</v>
@@ -3237,10 +3288,10 @@
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B181" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
       <c r="C181" t="s">
         <v>5</v>
@@ -3248,10 +3299,10 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B182" t="s">
-        <v>244</v>
+        <v>108</v>
       </c>
       <c r="C182" t="s">
         <v>5</v>
@@ -3259,10 +3310,10 @@
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B183" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C183" t="s">
         <v>5</v>
@@ -3270,10 +3321,10 @@
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B184" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C184" t="s">
         <v>5</v>
@@ -3281,10 +3332,10 @@
     </row>
     <row r="185">
       <c r="A185" t="s">
+        <v>260</v>
+      </c>
+      <c r="B185" t="s">
         <v>261</v>
-      </c>
-      <c r="B185" t="s">
-        <v>32</v>
       </c>
       <c r="C185" t="s">
         <v>5</v>
@@ -3295,7 +3346,7 @@
         <v>262</v>
       </c>
       <c r="B186" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="C186" t="s">
         <v>5</v>
@@ -3306,7 +3357,7 @@
         <v>263</v>
       </c>
       <c r="B187" t="s">
-        <v>244</v>
+        <v>153</v>
       </c>
       <c r="C187" t="s">
         <v>5</v>
@@ -3317,7 +3368,7 @@
         <v>264</v>
       </c>
       <c r="B188" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C188" t="s">
         <v>5</v>
@@ -3328,7 +3379,7 @@
         <v>265</v>
       </c>
       <c r="B189" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="C189" t="s">
         <v>5</v>
@@ -3336,10 +3387,10 @@
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B190" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C190" t="s">
         <v>5</v>
@@ -3347,10 +3398,10 @@
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B191" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="C191" t="s">
         <v>5</v>
@@ -3358,10 +3409,10 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B192" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="C192" t="s">
         <v>5</v>
@@ -3369,10 +3420,10 @@
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B193" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="C193" t="s">
         <v>5</v>
@@ -3380,10 +3431,10 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B194" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="C194" t="s">
         <v>5</v>
@@ -3391,10 +3442,10 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B195" t="s">
-        <v>21</v>
+        <v>132</v>
       </c>
       <c r="C195" t="s">
         <v>5</v>
@@ -3402,10 +3453,10 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B196" t="s">
-        <v>273</v>
+        <v>108</v>
       </c>
       <c r="C196" t="s">
         <v>5</v>
@@ -3416,7 +3467,7 @@
         <v>274</v>
       </c>
       <c r="B197" t="s">
-        <v>48</v>
+        <v>161</v>
       </c>
       <c r="C197" t="s">
         <v>5</v>
@@ -3427,7 +3478,7 @@
         <v>275</v>
       </c>
       <c r="B198" t="s">
-        <v>232</v>
+        <v>261</v>
       </c>
       <c r="C198" t="s">
         <v>5</v>
@@ -3438,7 +3489,7 @@
         <v>276</v>
       </c>
       <c r="B199" t="s">
-        <v>232</v>
+        <v>161</v>
       </c>
       <c r="C199" t="s">
         <v>5</v>
@@ -3449,7 +3500,7 @@
         <v>277</v>
       </c>
       <c r="B200" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="C200" t="s">
         <v>5</v>
@@ -3460,7 +3511,7 @@
         <v>278</v>
       </c>
       <c r="B201" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C201" t="s">
         <v>5</v>
@@ -3471,7 +3522,7 @@
         <v>279</v>
       </c>
       <c r="B202" t="s">
-        <v>23</v>
+        <v>153</v>
       </c>
       <c r="C202" t="s">
         <v>5</v>
@@ -3482,7 +3533,7 @@
         <v>280</v>
       </c>
       <c r="B203" t="s">
-        <v>23</v>
+        <v>261</v>
       </c>
       <c r="C203" t="s">
         <v>5</v>
@@ -3493,7 +3544,7 @@
         <v>281</v>
       </c>
       <c r="B204" t="s">
-        <v>126</v>
+        <v>14</v>
       </c>
       <c r="C204" t="s">
         <v>5</v>
@@ -3504,7 +3555,7 @@
         <v>282</v>
       </c>
       <c r="B205" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="C205" t="s">
         <v>5</v>
@@ -3515,7 +3566,7 @@
         <v>283</v>
       </c>
       <c r="B206" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C206" t="s">
         <v>5</v>
@@ -3526,7 +3577,7 @@
         <v>284</v>
       </c>
       <c r="B207" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C207" t="s">
         <v>5</v>
@@ -3537,7 +3588,7 @@
         <v>285</v>
       </c>
       <c r="B208" t="s">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="C208" t="s">
         <v>5</v>
@@ -3548,7 +3599,7 @@
         <v>286</v>
       </c>
       <c r="B209" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C209" t="s">
         <v>5</v>
@@ -3559,7 +3610,7 @@
         <v>287</v>
       </c>
       <c r="B210" t="s">
-        <v>39</v>
+        <v>137</v>
       </c>
       <c r="C210" t="s">
         <v>5</v>
@@ -3570,7 +3621,7 @@
         <v>288</v>
       </c>
       <c r="B211" t="s">
-        <v>126</v>
+        <v>14</v>
       </c>
       <c r="C211" t="s">
         <v>5</v>
@@ -3581,7 +3632,7 @@
         <v>289</v>
       </c>
       <c r="B212" t="s">
-        <v>39</v>
+        <v>290</v>
       </c>
       <c r="C212" t="s">
         <v>5</v>
@@ -3589,10 +3640,10 @@
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B213" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C213" t="s">
         <v>5</v>
@@ -3600,10 +3651,10 @@
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B214" t="s">
-        <v>54</v>
+        <v>249</v>
       </c>
       <c r="C214" t="s">
         <v>5</v>
@@ -3611,10 +3662,10 @@
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B215" t="s">
-        <v>293</v>
+        <v>249</v>
       </c>
       <c r="C215" t="s">
         <v>5</v>
@@ -3625,7 +3676,7 @@
         <v>294</v>
       </c>
       <c r="B216" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C216" t="s">
         <v>5</v>
@@ -3636,7 +3687,7 @@
         <v>295</v>
       </c>
       <c r="B217" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C217" t="s">
         <v>5</v>
@@ -3647,7 +3698,7 @@
         <v>296</v>
       </c>
       <c r="B218" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C218" t="s">
         <v>5</v>
@@ -3658,7 +3709,7 @@
         <v>297</v>
       </c>
       <c r="B219" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C219" t="s">
         <v>5</v>
@@ -3669,7 +3720,7 @@
         <v>298</v>
       </c>
       <c r="B220" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="C220" t="s">
         <v>5</v>
@@ -3680,7 +3731,7 @@
         <v>299</v>
       </c>
       <c r="B221" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C221" t="s">
         <v>5</v>
@@ -3691,7 +3742,7 @@
         <v>300</v>
       </c>
       <c r="B222" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C222" t="s">
         <v>5</v>
@@ -3702,7 +3753,7 @@
         <v>301</v>
       </c>
       <c r="B223" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C223" t="s">
         <v>5</v>
@@ -3713,7 +3764,7 @@
         <v>302</v>
       </c>
       <c r="B224" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C224" t="s">
         <v>5</v>
@@ -3724,9 +3775,185 @@
         <v>303</v>
       </c>
       <c r="B225" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="C225" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>304</v>
+      </c>
+      <c r="B226" t="s">
+        <v>62</v>
+      </c>
+      <c r="C226" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>305</v>
+      </c>
+      <c r="B227" t="s">
+        <v>144</v>
+      </c>
+      <c r="C227" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>306</v>
+      </c>
+      <c r="B228" t="s">
+        <v>62</v>
+      </c>
+      <c r="C228" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>307</v>
+      </c>
+      <c r="B229" t="s">
+        <v>28</v>
+      </c>
+      <c r="C229" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>308</v>
+      </c>
+      <c r="B230" t="s">
+        <v>77</v>
+      </c>
+      <c r="C230" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>309</v>
+      </c>
+      <c r="B231" t="s">
+        <v>310</v>
+      </c>
+      <c r="C231" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>311</v>
+      </c>
+      <c r="B232" t="s">
+        <v>37</v>
+      </c>
+      <c r="C232" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>312</v>
+      </c>
+      <c r="B233" t="s">
+        <v>85</v>
+      </c>
+      <c r="C233" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>313</v>
+      </c>
+      <c r="B234" t="s">
+        <v>85</v>
+      </c>
+      <c r="C234" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>314</v>
+      </c>
+      <c r="B235" t="s">
+        <v>88</v>
+      </c>
+      <c r="C235" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>315</v>
+      </c>
+      <c r="B236" t="s">
+        <v>85</v>
+      </c>
+      <c r="C236" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>316</v>
+      </c>
+      <c r="B237" t="s">
+        <v>85</v>
+      </c>
+      <c r="C237" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>317</v>
+      </c>
+      <c r="B238" t="s">
+        <v>31</v>
+      </c>
+      <c r="C238" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>318</v>
+      </c>
+      <c r="B239" t="s">
+        <v>31</v>
+      </c>
+      <c r="C239" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>319</v>
+      </c>
+      <c r="B240" t="s">
+        <v>31</v>
+      </c>
+      <c r="C240" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>320</v>
+      </c>
+      <c r="B241" t="s">
+        <v>31</v>
+      </c>
+      <c r="C241" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: update env and data
</commit_message>
<xml_diff>
--- a/data/GreatLink/GreatLink Asia Dividend Advantage.xlsx
+++ b/data/GreatLink/GreatLink Asia Dividend Advantage.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="PriceHistory" sheetId="1" r:id="GemRid910213"/>
+    <sheet name="PriceHistory" sheetId="1" r:id="GemRid630934"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="510">
   <si>
     <t>Price Date</t>
   </si>
@@ -26,15 +26,84 @@
     <t>Currency - Unit Level</t>
   </si>
   <si>
+    <t>04/11/2025</t>
+  </si>
+  <si>
+    <t>1.057</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>03/11/2025</t>
+  </si>
+  <si>
+    <t>1.063</t>
+  </si>
+  <si>
+    <t>31/10/2025</t>
+  </si>
+  <si>
+    <t>1.055</t>
+  </si>
+  <si>
+    <t>30/10/2025</t>
+  </si>
+  <si>
+    <t>1.058</t>
+  </si>
+  <si>
+    <t>29/10/2025</t>
+  </si>
+  <si>
+    <t>1.062</t>
+  </si>
+  <si>
+    <t>28/10/2025</t>
+  </si>
+  <si>
+    <t>1.051</t>
+  </si>
+  <si>
+    <t>27/10/2025</t>
+  </si>
+  <si>
+    <t>1.054</t>
+  </si>
+  <si>
+    <t>24/10/2025</t>
+  </si>
+  <si>
+    <t>23/10/2025</t>
+  </si>
+  <si>
+    <t>1.045</t>
+  </si>
+  <si>
+    <t>22/10/2025</t>
+  </si>
+  <si>
+    <t>1.046</t>
+  </si>
+  <si>
+    <t>21/10/2025</t>
+  </si>
+  <si>
+    <t>1.052</t>
+  </si>
+  <si>
+    <t>17/10/2025</t>
+  </si>
+  <si>
+    <t>1.024</t>
+  </si>
+  <si>
     <t>16/10/2025</t>
   </si>
   <si>
     <t>1.033</t>
   </si>
   <si>
-    <t>SGD</t>
-  </si>
-  <si>
     <t>15/10/2025</t>
   </si>
   <si>
@@ -60,9 +129,6 @@
   </si>
   <si>
     <t>09/10/2025</t>
-  </si>
-  <si>
-    <t>1.051</t>
   </si>
   <si>
     <t>08/10/2025</t>
@@ -1900,7 +1966,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1908,10 +1974,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -1919,10 +1985,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1930,10 +1996,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1941,10 +2007,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1952,10 +2018,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1963,10 +2029,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1999,7 +2065,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -2007,10 +2073,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -2018,10 +2084,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -2029,10 +2095,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2040,10 +2106,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -2051,10 +2117,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -2062,10 +2128,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -2073,10 +2139,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -2084,10 +2150,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -2095,10 +2161,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -2106,10 +2172,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -2117,10 +2183,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -2128,10 +2194,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -2139,10 +2205,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
@@ -2150,10 +2216,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -2161,10 +2227,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -2172,10 +2238,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -2183,10 +2249,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -2194,10 +2260,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -2205,10 +2271,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -2216,10 +2282,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -2241,7 +2307,7 @@
         <v>69</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -2249,10 +2315,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s">
         <v>71</v>
-      </c>
-      <c r="B41" t="s">
-        <v>59</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -2274,7 +2340,7 @@
         <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -2282,10 +2348,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -2293,10 +2359,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -2304,10 +2370,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -2315,10 +2381,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -2326,10 +2392,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -2337,10 +2403,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -2348,10 +2414,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -2359,10 +2425,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -2370,10 +2436,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -2381,10 +2447,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -2392,10 +2458,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -2403,10 +2469,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -2414,10 +2480,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -2425,10 +2491,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -2436,10 +2502,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -2447,10 +2513,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -2458,10 +2524,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -2469,10 +2535,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B61" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -2480,10 +2546,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -2491,10 +2557,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B63" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -2502,10 +2568,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -2513,10 +2579,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -2524,10 +2590,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -2535,10 +2601,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -2546,10 +2612,10 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B68" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -2557,10 +2623,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B69" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
@@ -2568,10 +2634,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B70" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -2579,10 +2645,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B71" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -2590,10 +2656,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B72" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -2601,7 +2667,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B73" t="s">
         <v>122</v>
@@ -2612,10 +2678,10 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B74" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
@@ -2623,10 +2689,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B75" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
@@ -2634,10 +2700,10 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="C76" t="s">
         <v>5</v>
@@ -2645,10 +2711,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B77" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C77" t="s">
         <v>5</v>
@@ -2656,10 +2722,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B78" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C78" t="s">
         <v>5</v>
@@ -2667,10 +2733,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B79" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C79" t="s">
         <v>5</v>
@@ -2678,10 +2744,10 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B80" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -2689,10 +2755,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="C81" t="s">
         <v>5</v>
@@ -2700,10 +2766,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B82" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
@@ -2711,10 +2777,10 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B83" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
@@ -2722,10 +2788,10 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B84" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="C84" t="s">
         <v>5</v>
@@ -2733,10 +2799,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B85" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C85" t="s">
         <v>5</v>
@@ -2744,10 +2810,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="C86" t="s">
         <v>5</v>
@@ -2755,10 +2821,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B87" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C87" t="s">
         <v>5</v>
@@ -2766,10 +2832,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B88" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="C88" t="s">
         <v>5</v>
@@ -2777,10 +2843,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B89" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
@@ -2788,10 +2854,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B90" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C90" t="s">
         <v>5</v>
@@ -2799,10 +2865,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B91" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
@@ -2810,10 +2876,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C92" t="s">
         <v>5</v>
@@ -2821,10 +2887,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B93" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C93" t="s">
         <v>5</v>
@@ -2832,10 +2898,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B94" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
@@ -2843,10 +2909,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B95" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C95" t="s">
         <v>5</v>
@@ -2854,10 +2920,10 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B96" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -2865,10 +2931,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B97" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
@@ -2876,10 +2942,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B98" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C98" t="s">
         <v>5</v>
@@ -2887,10 +2953,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B99" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
@@ -2898,10 +2964,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B100" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>
@@ -2909,10 +2975,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B101" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="C101" t="s">
         <v>5</v>
@@ -2920,10 +2986,10 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B102" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C102" t="s">
         <v>5</v>
@@ -2931,10 +2997,10 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B103" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
@@ -2942,10 +3008,10 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B104" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C104" t="s">
         <v>5</v>
@@ -2953,10 +3019,10 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="C105" t="s">
         <v>5</v>
@@ -2964,10 +3030,10 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B106" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="C106" t="s">
         <v>5</v>
@@ -2975,10 +3041,10 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
       <c r="C107" t="s">
         <v>5</v>
@@ -2986,10 +3052,10 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B108" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="C108" t="s">
         <v>5</v>
@@ -2997,10 +3063,10 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B109" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C109" t="s">
         <v>5</v>
@@ -3008,10 +3074,10 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B110" t="s">
-        <v>95</v>
+        <v>168</v>
       </c>
       <c r="C110" t="s">
         <v>5</v>
@@ -3019,10 +3085,10 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B111" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C111" t="s">
         <v>5</v>
@@ -3030,10 +3096,10 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B112" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C112" t="s">
         <v>5</v>
@@ -3041,10 +3107,10 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B113" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="C113" t="s">
         <v>5</v>
@@ -3052,10 +3118,10 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B114" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="C114" t="s">
         <v>5</v>
@@ -3063,10 +3129,10 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B115" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="C115" t="s">
         <v>5</v>
@@ -3074,10 +3140,10 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B116" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C116" t="s">
         <v>5</v>
@@ -3085,10 +3151,10 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B117" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="C117" t="s">
         <v>5</v>
@@ -3096,10 +3162,10 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="B118" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="C118" t="s">
         <v>5</v>
@@ -3107,10 +3173,10 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B119" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="C119" t="s">
         <v>5</v>
@@ -3118,10 +3184,10 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B120" t="s">
-        <v>181</v>
+        <v>117</v>
       </c>
       <c r="C120" t="s">
         <v>5</v>
@@ -3129,10 +3195,10 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B121" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C121" t="s">
         <v>5</v>
@@ -3140,10 +3206,10 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B122" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
       <c r="C122" t="s">
         <v>5</v>
@@ -3151,10 +3217,10 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B123" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="C123" t="s">
         <v>5</v>
@@ -3162,10 +3228,10 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B124" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C124" t="s">
         <v>5</v>
@@ -3173,10 +3239,10 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B125" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C125" t="s">
         <v>5</v>
@@ -3184,10 +3250,10 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B126" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="C126" t="s">
         <v>5</v>
@@ -3195,10 +3261,10 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B127" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C127" t="s">
         <v>5</v>
@@ -3206,10 +3272,10 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B128" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C128" t="s">
         <v>5</v>
@@ -3217,10 +3283,10 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B129" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C129" t="s">
         <v>5</v>
@@ -3228,10 +3294,10 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B130" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C130" t="s">
         <v>5</v>
@@ -3239,10 +3305,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
+        <v>206</v>
+      </c>
+      <c r="B131" t="s">
         <v>203</v>
-      </c>
-      <c r="B131" t="s">
-        <v>204</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -3250,10 +3316,10 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B132" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C132" t="s">
         <v>5</v>
@@ -3261,10 +3327,10 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B133" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C133" t="s">
         <v>5</v>
@@ -3272,10 +3338,10 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B134" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C134" t="s">
         <v>5</v>
@@ -3283,10 +3349,10 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B135" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C135" t="s">
         <v>5</v>
@@ -3294,10 +3360,10 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B136" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C136" t="s">
         <v>5</v>
@@ -3330,7 +3396,7 @@
         <v>219</v>
       </c>
       <c r="B139" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C139" t="s">
         <v>5</v>
@@ -3338,10 +3404,10 @@
     </row>
     <row r="140">
       <c r="A140" t="s">
+        <v>221</v>
+      </c>
+      <c r="B140" t="s">
         <v>220</v>
-      </c>
-      <c r="B140" t="s">
-        <v>111</v>
       </c>
       <c r="C140" t="s">
         <v>5</v>
@@ -3349,10 +3415,10 @@
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B141" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
       <c r="C141" t="s">
         <v>5</v>
@@ -3360,10 +3426,10 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B142" t="s">
-        <v>93</v>
+        <v>224</v>
       </c>
       <c r="C142" t="s">
         <v>5</v>
@@ -3371,10 +3437,10 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B143" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="C143" t="s">
         <v>5</v>
@@ -3382,10 +3448,10 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B144" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C144" t="s">
         <v>5</v>
@@ -3393,10 +3459,10 @@
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B145" t="s">
-        <v>154</v>
+        <v>230</v>
       </c>
       <c r="C145" t="s">
         <v>5</v>
@@ -3404,10 +3470,10 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B146" t="s">
-        <v>93</v>
+        <v>232</v>
       </c>
       <c r="C146" t="s">
         <v>5</v>
@@ -3415,10 +3481,10 @@
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B147" t="s">
-        <v>154</v>
+        <v>234</v>
       </c>
       <c r="C147" t="s">
         <v>5</v>
@@ -3426,10 +3492,10 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B148" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C148" t="s">
         <v>5</v>
@@ -3437,10 +3503,10 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B149" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="C149" t="s">
         <v>5</v>
@@ -3448,10 +3514,10 @@
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="B150" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="C150" t="s">
         <v>5</v>
@@ -3459,10 +3525,10 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B151" t="s">
-        <v>148</v>
+        <v>240</v>
       </c>
       <c r="C151" t="s">
         <v>5</v>
@@ -3470,10 +3536,10 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B152" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C152" t="s">
         <v>5</v>
@@ -3481,10 +3547,10 @@
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="B153" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="C153" t="s">
         <v>5</v>
@@ -3492,10 +3558,10 @@
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B154" t="s">
-        <v>238</v>
+        <v>115</v>
       </c>
       <c r="C154" t="s">
         <v>5</v>
@@ -3503,10 +3569,10 @@
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B155" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="C155" t="s">
         <v>5</v>
@@ -3514,10 +3580,10 @@
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B156" t="s">
-        <v>116</v>
+        <v>247</v>
       </c>
       <c r="C156" t="s">
         <v>5</v>
@@ -3525,10 +3591,10 @@
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="B157" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="C157" t="s">
         <v>5</v>
@@ -3536,10 +3602,10 @@
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="B158" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C158" t="s">
         <v>5</v>
@@ -3547,10 +3613,10 @@
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="B159" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
       <c r="C159" t="s">
         <v>5</v>
@@ -3558,10 +3624,10 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="B160" t="s">
-        <v>146</v>
+        <v>252</v>
       </c>
       <c r="C160" t="s">
         <v>5</v>
@@ -3569,10 +3635,10 @@
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="B161" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="C161" t="s">
         <v>5</v>
@@ -3580,10 +3646,10 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B162" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="C162" t="s">
         <v>5</v>
@@ -3591,10 +3657,10 @@
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B163" t="s">
-        <v>93</v>
+        <v>170</v>
       </c>
       <c r="C163" t="s">
         <v>5</v>
@@ -3602,10 +3668,10 @@
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B164" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C164" t="s">
         <v>5</v>
@@ -3613,10 +3679,10 @@
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="B165" t="s">
-        <v>120</v>
+        <v>258</v>
       </c>
       <c r="C165" t="s">
         <v>5</v>
@@ -3624,10 +3690,10 @@
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="B166" t="s">
-        <v>151</v>
+        <v>260</v>
       </c>
       <c r="C166" t="s">
         <v>5</v>
@@ -3635,10 +3701,10 @@
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="B167" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="C167" t="s">
         <v>5</v>
@@ -3646,10 +3712,10 @@
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="B168" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="C168" t="s">
         <v>5</v>
@@ -3657,10 +3723,10 @@
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="B169" t="s">
-        <v>89</v>
+        <v>178</v>
       </c>
       <c r="C169" t="s">
         <v>5</v>
@@ -3668,10 +3734,10 @@
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="B170" t="s">
-        <v>255</v>
+        <v>135</v>
       </c>
       <c r="C170" t="s">
         <v>5</v>
@@ -3679,10 +3745,10 @@
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="B171" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="C171" t="s">
         <v>5</v>
@@ -3690,10 +3756,10 @@
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="B172" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C172" t="s">
         <v>5</v>
@@ -3701,10 +3767,10 @@
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B173" t="s">
-        <v>116</v>
+        <v>260</v>
       </c>
       <c r="C173" t="s">
         <v>5</v>
@@ -3712,10 +3778,10 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="B174" t="s">
-        <v>163</v>
+        <v>260</v>
       </c>
       <c r="C174" t="s">
         <v>5</v>
@@ -3723,10 +3789,10 @@
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="B175" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C175" t="s">
         <v>5</v>
@@ -3734,10 +3800,10 @@
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="B176" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="C176" t="s">
         <v>5</v>
@@ -3745,10 +3811,10 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="B177" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="C177" t="s">
         <v>5</v>
@@ -3756,10 +3822,10 @@
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="B178" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
       <c r="C178" t="s">
         <v>5</v>
@@ -3767,10 +3833,10 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="B179" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="C179" t="s">
         <v>5</v>
@@ -3778,10 +3844,10 @@
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B180" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="C180" t="s">
         <v>5</v>
@@ -3789,10 +3855,10 @@
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="B181" t="s">
-        <v>267</v>
+        <v>111</v>
       </c>
       <c r="C181" t="s">
         <v>5</v>
@@ -3800,10 +3866,10 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B182" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C182" t="s">
         <v>5</v>
@@ -3811,10 +3877,10 @@
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B183" t="s">
-        <v>267</v>
+        <v>115</v>
       </c>
       <c r="C183" t="s">
         <v>5</v>
@@ -3822,10 +3888,10 @@
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B184" t="s">
-        <v>271</v>
+        <v>197</v>
       </c>
       <c r="C184" t="s">
         <v>5</v>
@@ -3833,10 +3899,10 @@
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="B185" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C185" t="s">
         <v>5</v>
@@ -3844,10 +3910,10 @@
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="B186" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="C186" t="s">
         <v>5</v>
@@ -3855,10 +3921,10 @@
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B187" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C187" t="s">
         <v>5</v>
@@ -3866,10 +3932,10 @@
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="B188" t="s">
-        <v>238</v>
+        <v>178</v>
       </c>
       <c r="C188" t="s">
         <v>5</v>
@@ -3877,10 +3943,10 @@
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="B189" t="s">
-        <v>146</v>
+        <v>197</v>
       </c>
       <c r="C189" t="s">
         <v>5</v>
@@ -3888,7 +3954,7 @@
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="B190" t="s">
         <v>146</v>
@@ -3899,10 +3965,10 @@
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B191" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="C191" t="s">
         <v>5</v>
@@ -3910,10 +3976,10 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="B192" t="s">
-        <v>280</v>
+        <v>146</v>
       </c>
       <c r="C192" t="s">
         <v>5</v>
@@ -3921,10 +3987,10 @@
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="B193" t="s">
-        <v>236</v>
+        <v>289</v>
       </c>
       <c r="C193" t="s">
         <v>5</v>
@@ -3932,10 +3998,10 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="B194" t="s">
-        <v>142</v>
+        <v>289</v>
       </c>
       <c r="C194" t="s">
         <v>5</v>
@@ -3943,10 +4009,10 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B195" t="s">
-        <v>124</v>
+        <v>289</v>
       </c>
       <c r="C195" t="s">
         <v>5</v>
@@ -3954,10 +4020,10 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="B196" t="s">
-        <v>175</v>
+        <v>293</v>
       </c>
       <c r="C196" t="s">
         <v>5</v>
@@ -3965,10 +4031,10 @@
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="B197" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="C197" t="s">
         <v>5</v>
@@ -3976,10 +4042,10 @@
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="B198" t="s">
-        <v>230</v>
+        <v>168</v>
       </c>
       <c r="C198" t="s">
         <v>5</v>
@@ -3987,10 +4053,10 @@
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="B199" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="C199" t="s">
         <v>5</v>
@@ -3998,10 +4064,10 @@
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="B200" t="s">
-        <v>100</v>
+        <v>260</v>
       </c>
       <c r="C200" t="s">
         <v>5</v>
@@ -4009,10 +4075,10 @@
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="B201" t="s">
-        <v>61</v>
+        <v>168</v>
       </c>
       <c r="C201" t="s">
         <v>5</v>
@@ -4020,10 +4086,10 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="B202" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
       <c r="C202" t="s">
         <v>5</v>
@@ -4031,10 +4097,10 @@
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="B203" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="C203" t="s">
         <v>5</v>
@@ -4042,10 +4108,10 @@
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="B204" t="s">
-        <v>53</v>
+        <v>302</v>
       </c>
       <c r="C204" t="s">
         <v>5</v>
@@ -4053,10 +4119,10 @@
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B205" t="s">
-        <v>53</v>
+        <v>258</v>
       </c>
       <c r="C205" t="s">
         <v>5</v>
@@ -4064,10 +4130,10 @@
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="B206" t="s">
-        <v>53</v>
+        <v>164</v>
       </c>
       <c r="C206" t="s">
         <v>5</v>
@@ -4075,10 +4141,10 @@
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="B207" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="C207" t="s">
         <v>5</v>
@@ -4086,10 +4152,10 @@
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="B208" t="s">
-        <v>83</v>
+        <v>197</v>
       </c>
       <c r="C208" t="s">
         <v>5</v>
@@ -4097,10 +4163,10 @@
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="B209" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C209" t="s">
         <v>5</v>
@@ -4108,10 +4174,10 @@
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="B210" t="s">
-        <v>80</v>
+        <v>252</v>
       </c>
       <c r="C210" t="s">
         <v>5</v>
@@ -4119,10 +4185,10 @@
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="B211" t="s">
-        <v>64</v>
+        <v>133</v>
       </c>
       <c r="C211" t="s">
         <v>5</v>
@@ -4130,10 +4196,10 @@
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="B212" t="s">
-        <v>301</v>
+        <v>122</v>
       </c>
       <c r="C212" t="s">
         <v>5</v>
@@ -4141,10 +4207,10 @@
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="B213" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C213" t="s">
         <v>5</v>
@@ -4152,10 +4218,10 @@
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="B214" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="C214" t="s">
         <v>5</v>
@@ -4163,10 +4229,10 @@
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="B215" t="s">
-        <v>305</v>
+        <v>126</v>
       </c>
       <c r="C215" t="s">
         <v>5</v>
@@ -4174,10 +4240,10 @@
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B216" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C216" t="s">
         <v>5</v>
@@ -4185,10 +4251,10 @@
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B217" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C217" t="s">
         <v>5</v>
@@ -4196,10 +4262,10 @@
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B218" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C218" t="s">
         <v>5</v>
@@ -4207,10 +4273,10 @@
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B219" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C219" t="s">
         <v>5</v>
@@ -4218,10 +4284,10 @@
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="B220" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="C220" t="s">
         <v>5</v>
@@ -4229,10 +4295,10 @@
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="B221" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="C221" t="s">
         <v>5</v>
@@ -4240,10 +4306,10 @@
     </row>
     <row r="222">
       <c r="A222" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="B222" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C222" t="s">
         <v>5</v>
@@ -4251,10 +4317,10 @@
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="B223" t="s">
-        <v>230</v>
+        <v>86</v>
       </c>
       <c r="C223" t="s">
         <v>5</v>
@@ -4262,10 +4328,10 @@
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="B224" t="s">
-        <v>111</v>
+        <v>323</v>
       </c>
       <c r="C224" t="s">
         <v>5</v>
@@ -4273,10 +4339,10 @@
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="B225" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C225" t="s">
         <v>5</v>
@@ -4284,10 +4350,10 @@
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="B226" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C226" t="s">
         <v>5</v>
@@ -4295,10 +4361,10 @@
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="B227" t="s">
-        <v>89</v>
+        <v>327</v>
       </c>
       <c r="C227" t="s">
         <v>5</v>
@@ -4306,10 +4372,10 @@
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="B228" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C228" t="s">
         <v>5</v>
@@ -4317,10 +4383,10 @@
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="B229" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="C229" t="s">
         <v>5</v>
@@ -4328,10 +4394,10 @@
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="B230" t="s">
-        <v>225</v>
+        <v>99</v>
       </c>
       <c r="C230" t="s">
         <v>5</v>
@@ -4339,10 +4405,10 @@
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="B231" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="C231" t="s">
         <v>5</v>
@@ -4350,10 +4416,10 @@
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="B232" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C232" t="s">
         <v>5</v>
@@ -4361,10 +4427,10 @@
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="B233" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C233" t="s">
         <v>5</v>
@@ -4372,10 +4438,10 @@
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="B234" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="C234" t="s">
         <v>5</v>
@@ -4383,10 +4449,10 @@
     </row>
     <row r="235">
       <c r="A235" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="B235" t="s">
-        <v>154</v>
+        <v>252</v>
       </c>
       <c r="C235" t="s">
         <v>5</v>
@@ -4394,10 +4460,10 @@
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="B236" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="C236" t="s">
         <v>5</v>
@@ -4405,10 +4471,10 @@
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="B237" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="C237" t="s">
         <v>5</v>
@@ -4416,10 +4482,10 @@
     </row>
     <row r="238">
       <c r="A238" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="B238" t="s">
-        <v>329</v>
+        <v>109</v>
       </c>
       <c r="C238" t="s">
         <v>5</v>
@@ -4427,10 +4493,10 @@
     </row>
     <row r="239">
       <c r="A239" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="B239" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="C239" t="s">
         <v>5</v>
@@ -4438,10 +4504,10 @@
     </row>
     <row r="240">
       <c r="A240" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="B240" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="C240" t="s">
         <v>5</v>
@@ -4449,10 +4515,10 @@
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="B241" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="C241" t="s">
         <v>5</v>
@@ -4460,10 +4526,10 @@
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="B242" t="s">
-        <v>175</v>
+        <v>247</v>
       </c>
       <c r="C242" t="s">
         <v>5</v>
@@ -4471,10 +4537,10 @@
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="B243" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="C243" t="s">
         <v>5</v>
@@ -4482,10 +4548,10 @@
     </row>
     <row r="244">
       <c r="A244" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="B244" t="s">
-        <v>230</v>
+        <v>117</v>
       </c>
       <c r="C244" t="s">
         <v>5</v>
@@ -4493,10 +4559,10 @@
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="B245" t="s">
-        <v>337</v>
+        <v>152</v>
       </c>
       <c r="C245" t="s">
         <v>5</v>
@@ -4504,10 +4570,10 @@
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="B246" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="C246" t="s">
         <v>5</v>
@@ -4515,10 +4581,10 @@
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="B247" t="s">
-        <v>85</v>
+        <v>176</v>
       </c>
       <c r="C247" t="s">
         <v>5</v>
@@ -4526,10 +4592,10 @@
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="B248" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="C248" t="s">
         <v>5</v>
@@ -4537,10 +4603,10 @@
     </row>
     <row r="249">
       <c r="A249" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B249" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C249" t="s">
         <v>5</v>
@@ -4548,10 +4614,10 @@
     </row>
     <row r="250">
       <c r="A250" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="B250" t="s">
-        <v>83</v>
+        <v>351</v>
       </c>
       <c r="C250" t="s">
         <v>5</v>
@@ -4559,10 +4625,10 @@
     </row>
     <row r="251">
       <c r="A251" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="B251" t="s">
-        <v>337</v>
+        <v>105</v>
       </c>
       <c r="C251" t="s">
         <v>5</v>
@@ -4570,10 +4636,10 @@
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="B252" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="C252" t="s">
         <v>5</v>
@@ -4581,10 +4647,10 @@
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="B253" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C253" t="s">
         <v>5</v>
@@ -4592,10 +4658,10 @@
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="B254" t="s">
-        <v>107</v>
+        <v>197</v>
       </c>
       <c r="C254" t="s">
         <v>5</v>
@@ -4603,10 +4669,10 @@
     </row>
     <row r="255">
       <c r="A255" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="B255" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="C255" t="s">
         <v>5</v>
@@ -4614,10 +4680,10 @@
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="B256" t="s">
-        <v>73</v>
+        <v>252</v>
       </c>
       <c r="C256" t="s">
         <v>5</v>
@@ -4625,10 +4691,10 @@
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="B257" t="s">
-        <v>80</v>
+        <v>359</v>
       </c>
       <c r="C257" t="s">
         <v>5</v>
@@ -4636,10 +4702,10 @@
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="B258" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="C258" t="s">
         <v>5</v>
@@ -4647,10 +4713,10 @@
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="B259" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="C259" t="s">
         <v>5</v>
@@ -4658,10 +4724,10 @@
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="B260" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="C260" t="s">
         <v>5</v>
@@ -4669,10 +4735,10 @@
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="B261" t="s">
-        <v>354</v>
+        <v>79</v>
       </c>
       <c r="C261" t="s">
         <v>5</v>
@@ -4680,10 +4746,10 @@
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="B262" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="C262" t="s">
         <v>5</v>
@@ -4691,10 +4757,10 @@
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="B263" t="s">
-        <v>66</v>
+        <v>359</v>
       </c>
       <c r="C263" t="s">
         <v>5</v>
@@ -4702,10 +4768,10 @@
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="B264" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C264" t="s">
         <v>5</v>
@@ -4713,10 +4779,10 @@
     </row>
     <row r="265">
       <c r="A265" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="B265" t="s">
-        <v>301</v>
+        <v>135</v>
       </c>
       <c r="C265" t="s">
         <v>5</v>
@@ -4724,10 +4790,10 @@
     </row>
     <row r="266">
       <c r="A266" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="B266" t="s">
-        <v>301</v>
+        <v>129</v>
       </c>
       <c r="C266" t="s">
         <v>5</v>
@@ -4735,10 +4801,10 @@
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="B267" t="s">
-        <v>305</v>
+        <v>122</v>
       </c>
       <c r="C267" t="s">
         <v>5</v>
@@ -4746,10 +4812,10 @@
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="B268" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C268" t="s">
         <v>5</v>
@@ -4757,10 +4823,10 @@
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="B269" t="s">
-        <v>175</v>
+        <v>102</v>
       </c>
       <c r="C269" t="s">
         <v>5</v>
@@ -4768,10 +4834,10 @@
     </row>
     <row r="270">
       <c r="A270" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="B270" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C270" t="s">
         <v>5</v>
@@ -4779,10 +4845,10 @@
     </row>
     <row r="271">
       <c r="A271" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="B271" t="s">
-        <v>126</v>
+        <v>79</v>
       </c>
       <c r="C271" t="s">
         <v>5</v>
@@ -4790,10 +4856,10 @@
     </row>
     <row r="272">
       <c r="A272" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="B272" t="s">
-        <v>238</v>
+        <v>83</v>
       </c>
       <c r="C272" t="s">
         <v>5</v>
@@ -4801,10 +4867,10 @@
     </row>
     <row r="273">
       <c r="A273" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B273" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="C273" t="s">
         <v>5</v>
@@ -4812,10 +4878,10 @@
     </row>
     <row r="274">
       <c r="A274" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="B274" t="s">
-        <v>369</v>
+        <v>71</v>
       </c>
       <c r="C274" t="s">
         <v>5</v>
@@ -4823,10 +4889,10 @@
     </row>
     <row r="275">
       <c r="A275" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="B275" t="s">
-        <v>371</v>
+        <v>88</v>
       </c>
       <c r="C275" t="s">
         <v>5</v>
@@ -4834,10 +4900,10 @@
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="B276" t="s">
-        <v>373</v>
+        <v>68</v>
       </c>
       <c r="C276" t="s">
         <v>5</v>
@@ -4845,10 +4911,10 @@
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="B277" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="C277" t="s">
         <v>5</v>
@@ -4856,10 +4922,10 @@
     </row>
     <row r="278">
       <c r="A278" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B278" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="C278" t="s">
         <v>5</v>
@@ -4867,10 +4933,10 @@
     </row>
     <row r="279">
       <c r="A279" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="B279" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="C279" t="s">
         <v>5</v>
@@ -4878,10 +4944,10 @@
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="B280" t="s">
-        <v>379</v>
+        <v>126</v>
       </c>
       <c r="C280" t="s">
         <v>5</v>
@@ -4889,10 +4955,10 @@
     </row>
     <row r="281">
       <c r="A281" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B281" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C281" t="s">
         <v>5</v>
@@ -4900,10 +4966,10 @@
     </row>
     <row r="282">
       <c r="A282" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="B282" t="s">
-        <v>379</v>
+        <v>117</v>
       </c>
       <c r="C282" t="s">
         <v>5</v>
@@ -4911,10 +4977,10 @@
     </row>
     <row r="283">
       <c r="A283" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B283" t="s">
-        <v>383</v>
+        <v>148</v>
       </c>
       <c r="C283" t="s">
         <v>5</v>
@@ -4922,10 +4988,10 @@
     </row>
     <row r="284">
       <c r="A284" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B284" t="s">
-        <v>383</v>
+        <v>260</v>
       </c>
       <c r="C284" t="s">
         <v>5</v>
@@ -4933,10 +4999,10 @@
     </row>
     <row r="285">
       <c r="A285" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B285" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C285" t="s">
         <v>5</v>
@@ -4944,10 +5010,10 @@
     </row>
     <row r="286">
       <c r="A286" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B286" t="s">
-        <v>367</v>
+        <v>391</v>
       </c>
       <c r="C286" t="s">
         <v>5</v>
@@ -4955,10 +5021,10 @@
     </row>
     <row r="287">
       <c r="A287" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="B287" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="C287" t="s">
         <v>5</v>
@@ -4966,10 +5032,10 @@
     </row>
     <row r="288">
       <c r="A288" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="B288" t="s">
-        <v>367</v>
+        <v>395</v>
       </c>
       <c r="C288" t="s">
         <v>5</v>
@@ -4977,10 +5043,10 @@
     </row>
     <row r="289">
       <c r="A289" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B289" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="C289" t="s">
         <v>5</v>
@@ -4988,10 +5054,10 @@
     </row>
     <row r="290">
       <c r="A290" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B290" t="s">
-        <v>183</v>
+        <v>395</v>
       </c>
       <c r="C290" t="s">
         <v>5</v>
@@ -4999,10 +5065,10 @@
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="B291" t="s">
-        <v>271</v>
+        <v>399</v>
       </c>
       <c r="C291" t="s">
         <v>5</v>
@@ -5010,10 +5076,10 @@
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="B292" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="C292" t="s">
         <v>5</v>
@@ -5021,10 +5087,10 @@
     </row>
     <row r="293">
       <c r="A293" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="B293" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="C293" t="s">
         <v>5</v>
@@ -5032,10 +5098,10 @@
     </row>
     <row r="294">
       <c r="A294" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B294" t="s">
-        <v>218</v>
+        <v>401</v>
       </c>
       <c r="C294" t="s">
         <v>5</v>
@@ -5043,10 +5109,10 @@
     </row>
     <row r="295">
       <c r="A295" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="B295" t="s">
-        <v>271</v>
+        <v>405</v>
       </c>
       <c r="C295" t="s">
         <v>5</v>
@@ -5054,10 +5120,10 @@
     </row>
     <row r="296">
       <c r="A296" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="B296" t="s">
-        <v>183</v>
+        <v>405</v>
       </c>
       <c r="C296" t="s">
         <v>5</v>
@@ -5065,10 +5131,10 @@
     </row>
     <row r="297">
       <c r="A297" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="B297" t="s">
-        <v>367</v>
+        <v>408</v>
       </c>
       <c r="C297" t="s">
         <v>5</v>
@@ -5076,10 +5142,10 @@
     </row>
     <row r="298">
       <c r="A298" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="B298" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C298" t="s">
         <v>5</v>
@@ -5087,10 +5153,10 @@
     </row>
     <row r="299">
       <c r="A299" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="B299" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="C299" t="s">
         <v>5</v>
@@ -5098,10 +5164,10 @@
     </row>
     <row r="300">
       <c r="A300" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B300" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="C300" t="s">
         <v>5</v>
@@ -5109,10 +5175,10 @@
     </row>
     <row r="301">
       <c r="A301" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="B301" t="s">
-        <v>383</v>
+        <v>413</v>
       </c>
       <c r="C301" t="s">
         <v>5</v>
@@ -5120,10 +5186,10 @@
     </row>
     <row r="302">
       <c r="A302" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="B302" t="s">
-        <v>408</v>
+        <v>205</v>
       </c>
       <c r="C302" t="s">
         <v>5</v>
@@ -5131,10 +5197,10 @@
     </row>
     <row r="303">
       <c r="A303" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="B303" t="s">
-        <v>410</v>
+        <v>293</v>
       </c>
       <c r="C303" t="s">
         <v>5</v>
@@ -5142,10 +5208,10 @@
     </row>
     <row r="304">
       <c r="A304" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="B304" t="s">
-        <v>198</v>
+        <v>417</v>
       </c>
       <c r="C304" t="s">
         <v>5</v>
@@ -5153,10 +5219,10 @@
     </row>
     <row r="305">
       <c r="A305" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="B305" t="s">
-        <v>377</v>
+        <v>200</v>
       </c>
       <c r="C305" t="s">
         <v>5</v>
@@ -5164,10 +5230,10 @@
     </row>
     <row r="306">
       <c r="A306" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="B306" t="s">
-        <v>377</v>
+        <v>240</v>
       </c>
       <c r="C306" t="s">
         <v>5</v>
@@ -5175,10 +5241,10 @@
     </row>
     <row r="307">
       <c r="A307" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="B307" t="s">
-        <v>415</v>
+        <v>293</v>
       </c>
       <c r="C307" t="s">
         <v>5</v>
@@ -5186,10 +5252,10 @@
     </row>
     <row r="308">
       <c r="A308" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B308" t="s">
-        <v>142</v>
+        <v>205</v>
       </c>
       <c r="C308" t="s">
         <v>5</v>
@@ -5197,10 +5263,10 @@
     </row>
     <row r="309">
       <c r="A309" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="B309" t="s">
-        <v>183</v>
+        <v>389</v>
       </c>
       <c r="C309" t="s">
         <v>5</v>
@@ -5208,10 +5274,10 @@
     </row>
     <row r="310">
       <c r="A310" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B310" t="s">
-        <v>139</v>
+        <v>405</v>
       </c>
       <c r="C310" t="s">
         <v>5</v>
@@ -5219,10 +5285,10 @@
     </row>
     <row r="311">
       <c r="A311" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="B311" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="C311" t="s">
         <v>5</v>
@@ -5230,10 +5296,10 @@
     </row>
     <row r="312">
       <c r="A312" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="B312" t="s">
-        <v>178</v>
+        <v>427</v>
       </c>
       <c r="C312" t="s">
         <v>5</v>
@@ -5241,10 +5307,10 @@
     </row>
     <row r="313">
       <c r="A313" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="B313" t="s">
-        <v>238</v>
+        <v>405</v>
       </c>
       <c r="C313" t="s">
         <v>5</v>
@@ -5252,10 +5318,10 @@
     </row>
     <row r="314">
       <c r="A314" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="B314" t="s">
-        <v>175</v>
+        <v>430</v>
       </c>
       <c r="C314" t="s">
         <v>5</v>
@@ -5263,10 +5329,10 @@
     </row>
     <row r="315">
       <c r="A315" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="B315" t="s">
-        <v>175</v>
+        <v>432</v>
       </c>
       <c r="C315" t="s">
         <v>5</v>
@@ -5274,10 +5340,10 @@
     </row>
     <row r="316">
       <c r="A316" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="B316" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
       <c r="C316" t="s">
         <v>5</v>
@@ -5285,10 +5351,10 @@
     </row>
     <row r="317">
       <c r="A317" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="B317" t="s">
-        <v>83</v>
+        <v>399</v>
       </c>
       <c r="C317" t="s">
         <v>5</v>
@@ -5296,10 +5362,10 @@
     </row>
     <row r="318">
       <c r="A318" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="B318" t="s">
-        <v>337</v>
+        <v>399</v>
       </c>
       <c r="C318" t="s">
         <v>5</v>
@@ -5307,10 +5373,10 @@
     </row>
     <row r="319">
       <c r="A319" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="B319" t="s">
-        <v>100</v>
+        <v>437</v>
       </c>
       <c r="C319" t="s">
         <v>5</v>
@@ -5318,10 +5384,10 @@
     </row>
     <row r="320">
       <c r="A320" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="B320" t="s">
-        <v>59</v>
+        <v>164</v>
       </c>
       <c r="C320" t="s">
         <v>5</v>
@@ -5329,10 +5395,10 @@
     </row>
     <row r="321">
       <c r="A321" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="B321" t="s">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="C321" t="s">
         <v>5</v>
@@ -5340,10 +5406,10 @@
     </row>
     <row r="322">
       <c r="A322" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="B322" t="s">
-        <v>329</v>
+        <v>161</v>
       </c>
       <c r="C322" t="s">
         <v>5</v>
@@ -5351,10 +5417,10 @@
     </row>
     <row r="323">
       <c r="A323" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="B323" t="s">
-        <v>255</v>
+        <v>442</v>
       </c>
       <c r="C323" t="s">
         <v>5</v>
@@ -5362,10 +5428,10 @@
     </row>
     <row r="324">
       <c r="A324" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="B324" t="s">
-        <v>434</v>
+        <v>200</v>
       </c>
       <c r="C324" t="s">
         <v>5</v>
@@ -5373,10 +5439,10 @@
     </row>
     <row r="325">
       <c r="A325" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="B325" t="s">
-        <v>107</v>
+        <v>260</v>
       </c>
       <c r="C325" t="s">
         <v>5</v>
@@ -5384,10 +5450,10 @@
     </row>
     <row r="326">
       <c r="A326" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
       <c r="B326" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="C326" t="s">
         <v>5</v>
@@ -5395,10 +5461,10 @@
     </row>
     <row r="327">
       <c r="A327" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="B327" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
       <c r="C327" t="s">
         <v>5</v>
@@ -5406,10 +5472,10 @@
     </row>
     <row r="328">
       <c r="A328" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
       <c r="B328" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="C328" t="s">
         <v>5</v>
@@ -5417,10 +5483,10 @@
     </row>
     <row r="329">
       <c r="A329" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="B329" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C329" t="s">
         <v>5</v>
@@ -5428,10 +5494,10 @@
     </row>
     <row r="330">
       <c r="A330" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="B330" t="s">
-        <v>85</v>
+        <v>359</v>
       </c>
       <c r="C330" t="s">
         <v>5</v>
@@ -5439,10 +5505,10 @@
     </row>
     <row r="331">
       <c r="A331" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="B331" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="C331" t="s">
         <v>5</v>
@@ -5450,10 +5516,10 @@
     </row>
     <row r="332">
       <c r="A332" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="B332" t="s">
-        <v>337</v>
+        <v>81</v>
       </c>
       <c r="C332" t="s">
         <v>5</v>
@@ -5461,10 +5527,10 @@
     </row>
     <row r="333">
       <c r="A333" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="B333" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
       <c r="C333" t="s">
         <v>5</v>
@@ -5472,10 +5538,10 @@
     </row>
     <row r="334">
       <c r="A334" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="B334" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="C334" t="s">
         <v>5</v>
@@ -5483,10 +5549,10 @@
     </row>
     <row r="335">
       <c r="A335" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="B335" t="s">
-        <v>87</v>
+        <v>277</v>
       </c>
       <c r="C335" t="s">
         <v>5</v>
@@ -5494,10 +5560,10 @@
     </row>
     <row r="336">
       <c r="A336" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="B336" t="s">
-        <v>89</v>
+        <v>456</v>
       </c>
       <c r="C336" t="s">
         <v>5</v>
@@ -5505,10 +5571,10 @@
     </row>
     <row r="337">
       <c r="A337" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="B337" t="s">
-        <v>329</v>
+        <v>129</v>
       </c>
       <c r="C337" t="s">
         <v>5</v>
@@ -5516,10 +5582,10 @@
     </row>
     <row r="338">
       <c r="A338" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="B338" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="C338" t="s">
         <v>5</v>
@@ -5527,10 +5593,10 @@
     </row>
     <row r="339">
       <c r="A339" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="B339" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C339" t="s">
         <v>5</v>
@@ -5538,10 +5604,10 @@
     </row>
     <row r="340">
       <c r="A340" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="B340" t="s">
-        <v>87</v>
+        <v>247</v>
       </c>
       <c r="C340" t="s">
         <v>5</v>
@@ -5549,10 +5615,10 @@
     </row>
     <row r="341">
       <c r="A341" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
       <c r="B341" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="C341" t="s">
         <v>5</v>
@@ -5560,10 +5626,10 @@
     </row>
     <row r="342">
       <c r="A342" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="B342" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="C342" t="s">
         <v>5</v>
@@ -5571,10 +5637,10 @@
     </row>
     <row r="343">
       <c r="A343" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="B343" t="s">
-        <v>175</v>
+        <v>105</v>
       </c>
       <c r="C343" t="s">
         <v>5</v>
@@ -5582,10 +5648,10 @@
     </row>
     <row r="344">
       <c r="A344" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="B344" t="s">
-        <v>91</v>
+        <v>359</v>
       </c>
       <c r="C344" t="s">
         <v>5</v>
@@ -5593,10 +5659,10 @@
     </row>
     <row r="345">
       <c r="A345" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="B345" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C345" t="s">
         <v>5</v>
@@ -5604,10 +5670,10 @@
     </row>
     <row r="346">
       <c r="A346" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="B346" t="s">
-        <v>93</v>
+        <v>359</v>
       </c>
       <c r="C346" t="s">
         <v>5</v>
@@ -5615,10 +5681,10 @@
     </row>
     <row r="347">
       <c r="A347" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="B347" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="C347" t="s">
         <v>5</v>
@@ -5626,10 +5692,10 @@
     </row>
     <row r="348">
       <c r="A348" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
       <c r="B348" t="s">
-        <v>267</v>
+        <v>111</v>
       </c>
       <c r="C348" t="s">
         <v>5</v>
@@ -5637,10 +5703,10 @@
     </row>
     <row r="349">
       <c r="A349" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="B349" t="s">
-        <v>139</v>
+        <v>351</v>
       </c>
       <c r="C349" t="s">
         <v>5</v>
@@ -5648,10 +5714,10 @@
     </row>
     <row r="350">
       <c r="A350" t="s">
-        <v>460</v>
+        <v>470</v>
       </c>
       <c r="B350" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="C350" t="s">
         <v>5</v>
@@ -5659,10 +5725,10 @@
     </row>
     <row r="351">
       <c r="A351" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="B351" t="s">
-        <v>280</v>
+        <v>115</v>
       </c>
       <c r="C351" t="s">
         <v>5</v>
@@ -5670,10 +5736,10 @@
     </row>
     <row r="352">
       <c r="A352" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
       <c r="B352" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="C352" t="s">
         <v>5</v>
@@ -5681,10 +5747,10 @@
     </row>
     <row r="353">
       <c r="A353" t="s">
-        <v>463</v>
+        <v>473</v>
       </c>
       <c r="B353" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C353" t="s">
         <v>5</v>
@@ -5692,10 +5758,10 @@
     </row>
     <row r="354">
       <c r="A354" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="B354" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C354" t="s">
         <v>5</v>
@@ -5703,10 +5769,10 @@
     </row>
     <row r="355">
       <c r="A355" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="B355" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="C355" t="s">
         <v>5</v>
@@ -5714,7 +5780,7 @@
     </row>
     <row r="356">
       <c r="A356" t="s">
-        <v>466</v>
+        <v>476</v>
       </c>
       <c r="B356" t="s">
         <v>113</v>
@@ -5725,10 +5791,10 @@
     </row>
     <row r="357">
       <c r="A357" t="s">
-        <v>467</v>
+        <v>477</v>
       </c>
       <c r="B357" t="s">
-        <v>163</v>
+        <v>109</v>
       </c>
       <c r="C357" t="s">
         <v>5</v>
@@ -5736,10 +5802,10 @@
     </row>
     <row r="358">
       <c r="A358" t="s">
-        <v>468</v>
+        <v>478</v>
       </c>
       <c r="B358" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="C358" t="s">
         <v>5</v>
@@ -5747,10 +5813,10 @@
     </row>
     <row r="359">
       <c r="A359" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="B359" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C359" t="s">
         <v>5</v>
@@ -5758,10 +5824,10 @@
     </row>
     <row r="360">
       <c r="A360" t="s">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="B360" t="s">
-        <v>91</v>
+        <v>289</v>
       </c>
       <c r="C360" t="s">
         <v>5</v>
@@ -5769,10 +5835,10 @@
     </row>
     <row r="361">
       <c r="A361" t="s">
-        <v>471</v>
+        <v>481</v>
       </c>
       <c r="B361" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C361" t="s">
         <v>5</v>
@@ -5780,10 +5846,10 @@
     </row>
     <row r="362">
       <c r="A362" t="s">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="B362" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="C362" t="s">
         <v>5</v>
@@ -5791,10 +5857,10 @@
     </row>
     <row r="363">
       <c r="A363" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="B363" t="s">
-        <v>163</v>
+        <v>302</v>
       </c>
       <c r="C363" t="s">
         <v>5</v>
@@ -5802,10 +5868,10 @@
     </row>
     <row r="364">
       <c r="A364" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="B364" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="C364" t="s">
         <v>5</v>
@@ -5813,10 +5879,10 @@
     </row>
     <row r="365">
       <c r="A365" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="B365" t="s">
-        <v>126</v>
+        <v>197</v>
       </c>
       <c r="C365" t="s">
         <v>5</v>
@@ -5824,10 +5890,10 @@
     </row>
     <row r="366">
       <c r="A366" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="B366" t="s">
-        <v>477</v>
+        <v>197</v>
       </c>
       <c r="C366" t="s">
         <v>5</v>
@@ -5835,10 +5901,10 @@
     </row>
     <row r="367">
       <c r="A367" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="B367" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C367" t="s">
         <v>5</v>
@@ -5846,10 +5912,10 @@
     </row>
     <row r="368">
       <c r="A368" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
       <c r="B368" t="s">
-        <v>280</v>
+        <v>135</v>
       </c>
       <c r="C368" t="s">
         <v>5</v>
@@ -5857,10 +5923,10 @@
     </row>
     <row r="369">
       <c r="A369" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
       <c r="B369" t="s">
-        <v>280</v>
+        <v>185</v>
       </c>
       <c r="C369" t="s">
         <v>5</v>
@@ -5868,10 +5934,10 @@
     </row>
     <row r="370">
       <c r="A370" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
       <c r="B370" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="C370" t="s">
         <v>5</v>
@@ -5879,10 +5945,10 @@
     </row>
     <row r="371">
       <c r="A371" t="s">
-        <v>482</v>
+        <v>491</v>
       </c>
       <c r="B371" t="s">
-        <v>280</v>
+        <v>176</v>
       </c>
       <c r="C371" t="s">
         <v>5</v>
@@ -5890,10 +5956,10 @@
     </row>
     <row r="372">
       <c r="A372" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="B372" t="s">
-        <v>280</v>
+        <v>113</v>
       </c>
       <c r="C372" t="s">
         <v>5</v>
@@ -5901,10 +5967,10 @@
     </row>
     <row r="373">
       <c r="A373" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
       <c r="B373" t="s">
-        <v>236</v>
+        <v>185</v>
       </c>
       <c r="C373" t="s">
         <v>5</v>
@@ -5912,10 +5978,10 @@
     </row>
     <row r="374">
       <c r="A374" t="s">
-        <v>485</v>
+        <v>494</v>
       </c>
       <c r="B374" t="s">
-        <v>236</v>
+        <v>117</v>
       </c>
       <c r="C374" t="s">
         <v>5</v>
@@ -5923,10 +5989,10 @@
     </row>
     <row r="375">
       <c r="A375" t="s">
-        <v>486</v>
+        <v>495</v>
       </c>
       <c r="B375" t="s">
-        <v>236</v>
+        <v>185</v>
       </c>
       <c r="C375" t="s">
         <v>5</v>
@@ -5934,12 +6000,144 @@
     </row>
     <row r="376">
       <c r="A376" t="s">
-        <v>487</v>
+        <v>496</v>
       </c>
       <c r="B376" t="s">
-        <v>236</v>
+        <v>170</v>
       </c>
       <c r="C376" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="s">
+        <v>497</v>
+      </c>
+      <c r="B377" t="s">
+        <v>148</v>
+      </c>
+      <c r="C377" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="s">
+        <v>498</v>
+      </c>
+      <c r="B378" t="s">
+        <v>499</v>
+      </c>
+      <c r="C378" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="s">
+        <v>500</v>
+      </c>
+      <c r="B379" t="s">
+        <v>138</v>
+      </c>
+      <c r="C379" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="s">
+        <v>501</v>
+      </c>
+      <c r="B380" t="s">
+        <v>302</v>
+      </c>
+      <c r="C380" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="s">
+        <v>502</v>
+      </c>
+      <c r="B381" t="s">
+        <v>302</v>
+      </c>
+      <c r="C381" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="s">
+        <v>503</v>
+      </c>
+      <c r="B382" t="s">
+        <v>164</v>
+      </c>
+      <c r="C382" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="s">
+        <v>504</v>
+      </c>
+      <c r="B383" t="s">
+        <v>302</v>
+      </c>
+      <c r="C383" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="s">
+        <v>505</v>
+      </c>
+      <c r="B384" t="s">
+        <v>302</v>
+      </c>
+      <c r="C384" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="s">
+        <v>506</v>
+      </c>
+      <c r="B385" t="s">
+        <v>258</v>
+      </c>
+      <c r="C385" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="s">
+        <v>507</v>
+      </c>
+      <c r="B386" t="s">
+        <v>258</v>
+      </c>
+      <c r="C386" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="s">
+        <v>508</v>
+      </c>
+      <c r="B387" t="s">
+        <v>258</v>
+      </c>
+      <c r="C387" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="s">
+        <v>509</v>
+      </c>
+      <c r="B388" t="s">
+        <v>258</v>
+      </c>
+      <c r="C388" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>